<commit_message>
lesson-5 fixed with extra material about functions
</commit_message>
<xml_diff>
--- a/Программа курса.xlsx
+++ b/Программа курса.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\courses\python_Boot_camp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC285CD-BB66-40D5-B5D8-CBB9932B9853}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D2994E-FCA0-408A-BA70-71F168BC4F63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1200" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Установка ПО. Примеры применения</t>
   </si>
@@ -130,9 +130,9 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Примеры работы с функциями и задачи на понимание областей видимости. </t>
-    </r>
+    <t xml:space="preserve">Работа со строками, байтами, кодировками. Модули io, chardet, zipfile, random. Открытие и закрытие файлов. Оператор with. Форматирование строк. </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -142,11 +142,188 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Генерирование рандомных параметров для автозаполнения</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Работа со строками, байтами, кодировками. Модули io, chardet, zipfile, random. Открытие и закрытие файлов. Оператор with. Форматирование строк. </t>
+      <t>Отладка в VSC,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Задачи, содержащие цикл, условные конструкции, цикл в цикле, операторы, работающие внутри цикла. Базовые методы строк. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Импортирование модулей и пакетов. Способы создания. Конфигурация VSC. Документирование. Настройка виртуального окружения. Импортирование пакетов. </t>
+  </si>
+  <si>
+    <t>Модуль 5. Инструменты функционального программирования</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Подсчет running average. Создание декаратора для определения времени выполнения функции.  </t>
+  </si>
+  <si>
+    <t>Модуль 6. ООП</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Функции обратного вызова. Функции высших порядков. Встроенные функции высших порядков. Генерация функций. Списки функций. Списковые включения. Лямбда функции. Модуль functools, operator. Partial functions. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Использование инструментов функционального программирования. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Monkey patching. </t>
+    </r>
+  </si>
+  <si>
+    <t>Модуль 8. Параллельные вычисления</t>
+  </si>
+  <si>
+    <t>Модуль 7. Библотеки для работы с ресурсами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Классы, объекты.  Методы, атрибуты. Проектирование классов. self. Доступ к атрибутам(getattr, setattr,hasattr). Создание копий объекта. Наследование . super. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создание класса Car. Создание иерархии классов на основе класса Figure. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collections. Slice. Decimal, json, xml, yaml, date, time, datetime, re </t>
+  </si>
+  <si>
+    <t>Работа с различными типами данных, различными файлами и с регулярными выражениями</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Многопоточность. </t>
+  </si>
+  <si>
+    <t>Многопроцессороное программирование. Futures</t>
+  </si>
+  <si>
+    <t>Deadlock, Daemons, Multiprocessing</t>
+  </si>
+  <si>
+    <t>Примитивы синхронизации, Очереди, Блокировки</t>
+  </si>
+  <si>
+    <t>Asyncio. Aiohttp, requests, beautifulsoup</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asyncio examples. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Парсинг сайта</t>
+    </r>
+  </si>
+  <si>
+    <t>Модуль 9. Анализ данных</t>
+  </si>
+  <si>
+    <t>Модуль Numpy. Базовый функционал. Визуализация данных. Базовый функционал.</t>
+  </si>
+  <si>
+    <t>Модуль Pandas. Базовый функционал. Визуализация данных.</t>
+  </si>
+  <si>
+    <t>Базовый синтаксис при работе с numpy, matplotlib</t>
+  </si>
+  <si>
+    <t>Базовый синтаксис при работе с pandas, matplotlib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Замыкания. Генераторы. Декораторы.  Nonlocal. Ленивые вычисления. </t>
+  </si>
+  <si>
+    <t>Модуль 10. Тестирование</t>
+  </si>
+  <si>
+    <t>Написание логов</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Логирование, logging. ООП декораторы @property, @staticmethod, @classmethod</t>
+  </si>
+  <si>
+    <t>Тестирование, unittest. Mock</t>
+  </si>
+  <si>
+    <t>Написание тестов.</t>
+  </si>
+  <si>
+    <t>Работа с WEB API, smtp</t>
+  </si>
+  <si>
+    <t>Отправление email, работа с youtube api, openweather api, Postman</t>
+  </si>
+  <si>
+    <t>Модуль 11. Flask</t>
+  </si>
+  <si>
+    <t>Введение во flask, routing, forms</t>
+  </si>
+  <si>
+    <t>Создание приложения</t>
+  </si>
+  <si>
+    <t>Работа с ORM SQLALCHEMY</t>
+  </si>
+  <si>
+    <t>Tkinter app</t>
+  </si>
+  <si>
+    <t>Tkinter, Перегрузка арифметических магических методов.</t>
+  </si>
+  <si>
+    <t>Абстрактные методы. Миксины. SOLID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Множественное наследование, Meta classes</t>
+  </si>
+  <si>
+    <t>Примеры использования</t>
+  </si>
+  <si>
+    <t>Модуль 12. NoSQL</t>
+  </si>
+  <si>
+    <t>Введение в MongoDB</t>
+  </si>
+  <si>
+    <t>Создание простого приложение и использованием mongoengine</t>
+  </si>
+  <si>
+    <t>. Словари. Множества. Методы последовательностей. Распаковка. Модули json, difflib</t>
+  </si>
+  <si>
+    <t>Базовые конструкции. Переменные. Циклы. Ветвление. Инструменты отладки. Работа со строками. Базовые операции со строками. Индексация. Методы. Форматирование. Списки. Диапозоны. Кортежи</t>
+  </si>
+  <si>
+    <t>Авторизация, Swagger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модуль 2. Работа с файлами, директориями и форматирование. </t>
+  </si>
+  <si>
+    <t>Модули os и os.path. Обход директорий. Работа с файлами и папками. Передача аргументов командной строки. Позиционирование в файле. Модуль io, pyinstaller, shutil.  *Блокировщик сайтов. Создание функций. Области видимости. Глобальные и локальные переменные. Возвращение значений. Обязательные и необязательные параметры. global. Передача аргументов по имени, позиции.  Is, ==.</t>
   </si>
   <si>
     <r>
@@ -173,6 +350,14 @@
       </rPr>
       <t xml:space="preserve">. </t>
     </r>
+  </si>
+  <si>
+    <t>Рекурсия. Хранение базовых структур в памяти. Изменяемые и неизменяемые типы. Глубокие и поверхностные копии. Модуль copy.  Виды стандартных исключений. Обработка исключений. Инструкции try, except, else, finally. Модуль warning. Assert. Eval. Модуль functools.  *Модуль faker</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Примеры работы с функциями и задачи на понимание областей видимости. Генерирование рандомных параметров для автозаполнения. Визуализация хранения переменных в памяти. </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -182,16 +367,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Блокировщик сайтов</t>
-    </r>
-  </si>
-  <si>
-    <t>Модули os и os.path. Обход директорий. Работа с файлами и папками. Передача аргументов командной строки. Позиционирование в файле. Модуль io, pyinstaller, shutil.  *Блокировщик сайтов</t>
-  </si>
-  <si>
-    <t>Создание функций. Области видимости. Глобальные и локальные переменные. Возвращение значений. Обязательные и необязательные параметры. global. Передача аргументов по имени, позиции.  Is, ==. *Модуль faker</t>
-  </si>
-  <si>
+      <t>Stack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -201,25 +388,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Отладка в VSC,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Задачи, содержащие цикл, условные конструкции, цикл в цикле, операторы, работающие внутри цикла. Базовые методы строк. </t>
-    </r>
-  </si>
-  <si>
-    <t>Рекурсия. Хранение базовых структур в памяти. Изменяемые и неизменяемые типы. Глубокие и поверхностные копии. Модуль copy.  Виды стандартных исключений. Обработка исключений. Инструкции try, except, else, finally. Модуль warning. Assert. Eval. Модуль functools</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Визуализация хранения переменных в памяти. </t>
+      <t xml:space="preserve">Assert. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Работа с исключениями. </t>
     </r>
     <r>
       <rPr>
@@ -230,214 +409,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Stack</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Assert. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Работа с исключениями. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Мемоизация</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Импортирование модулей и пакетов. Способы создания. Конфигурация VSC. Документирование. Настройка виртуального окружения. Импортирование пакетов. </t>
-  </si>
-  <si>
-    <t>Модуль 5. Инструменты функционального программирования</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Подсчет running average. Создание декаратора для определения времени выполнения функции.  </t>
-  </si>
-  <si>
-    <t>Модуль 6. ООП</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Функции обратного вызова. Функции высших порядков. Встроенные функции высших порядков. Генерация функций. Списки функций. Списковые включения. Лямбда функции. Модуль functools, operator. Partial functions. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Использование инструментов функционального программирования. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Monkey patching. </t>
-    </r>
-  </si>
-  <si>
-    <t>Модуль 8. Параллельные вычисления</t>
-  </si>
-  <si>
-    <t>Модуль 7. Библотеки для работы с ресурсами</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Классы, объекты.  Методы, атрибуты. Проектирование классов. self. Доступ к атрибутам(getattr, setattr,hasattr). Создание копий объекта. Наследование . super. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Создание класса Car. Создание иерархии классов на основе класса Figure. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collections. Slice. Decimal, json, xml, yaml, date, time, datetime, re </t>
-  </si>
-  <si>
-    <t>Работа с различными типами данных, различными файлами и с регулярными выражениями</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Многопоточность. </t>
-  </si>
-  <si>
-    <t>Многопроцессороное программирование. Futures</t>
-  </si>
-  <si>
-    <t>Deadlock, Daemons, Multiprocessing</t>
-  </si>
-  <si>
-    <t>Примитивы синхронизации, Очереди, Блокировки</t>
-  </si>
-  <si>
-    <t>Asyncio. Aiohttp, requests, beautifulsoup</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Asyncio examples. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Парсинг сайта</t>
-    </r>
-  </si>
-  <si>
-    <t>Модуль 9. Анализ данных</t>
-  </si>
-  <si>
-    <t>Модуль Numpy. Базовый функционал. Визуализация данных. Базовый функционал.</t>
-  </si>
-  <si>
-    <t>Модуль Pandas. Базовый функционал. Визуализация данных.</t>
-  </si>
-  <si>
-    <t>Базовый синтаксис при работе с numpy, matplotlib</t>
-  </si>
-  <si>
-    <t>Базовый синтаксис при работе с pandas, matplotlib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Замыкания. Генераторы. Декораторы.  Nonlocal. Ленивые вычисления. </t>
-  </si>
-  <si>
-    <t>Модуль 10. Тестирование</t>
-  </si>
-  <si>
-    <t>Написание логов</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Логирование, logging. ООП декораторы @property, @staticmethod, @classmethod</t>
-  </si>
-  <si>
-    <t>Тестирование, unittest. Mock</t>
-  </si>
-  <si>
-    <t>Написание тестов.</t>
-  </si>
-  <si>
-    <t>Работа с WEB API, smtp</t>
-  </si>
-  <si>
-    <t>Отправление email, работа с youtube api, openweather api, Postman</t>
-  </si>
-  <si>
-    <t>Модуль 11. Flask</t>
-  </si>
-  <si>
-    <t>Введение во flask, routing, forms</t>
-  </si>
-  <si>
-    <t>Создание приложения</t>
-  </si>
-  <si>
-    <t>Работа с ORM SQLALCHEMY</t>
-  </si>
-  <si>
-    <t>Tkinter app</t>
-  </si>
-  <si>
-    <t>Tkinter, Перегрузка арифметических магических методов.</t>
-  </si>
-  <si>
-    <t>Абстрактные методы. Миксины. SOLID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Множественное наследование, Meta classes</t>
-  </si>
-  <si>
-    <t>Примеры использования</t>
-  </si>
-  <si>
-    <t>Модуль 12. NoSQL</t>
-  </si>
-  <si>
-    <t>Введение в MongoDB</t>
-  </si>
-  <si>
-    <t>Создание простого приложение и использованием mongoengine</t>
-  </si>
-  <si>
-    <t>. Словари. Множества. Методы последовательностей. Распаковка. Модули json, difflib</t>
-  </si>
-  <si>
-    <t>Базовые конструкции. Переменные. Циклы. Ветвление. Инструменты отладки. Работа со строками. Базовые операции со строками. Индексация. Методы. Форматирование. Списки. Диапозоны. Кортежи</t>
-  </si>
-  <si>
-    <t>Авторизация, Swagger</t>
   </si>
 </sst>
 </file>
@@ -802,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,10 +810,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -852,7 +825,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -867,7 +840,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -876,76 +849,76 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -954,43 +927,43 @@
     <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -999,13 +972,13 @@
     <row r="13" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1014,28 +987,28 @@
     <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1044,13 +1017,13 @@
     <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1064,8 +1037,8 @@
       <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>40</v>
+      <c r="D17" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1074,13 +1047,13 @@
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1089,28 +1062,28 @@
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="E19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1119,13 +1092,13 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1134,13 +1107,13 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1149,13 +1122,13 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1164,13 +1137,13 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1179,13 +1152,13 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1194,13 +1167,13 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1208,34 +1181,19 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>